<commit_message>
Database Schema Modified By Pratik
</commit_message>
<xml_diff>
--- a/doc/Database schema.xlsx
+++ b/doc/Database schema.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pratik CDAC\Project\Online-Bidding-system-Group-19-Project\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDD9BD-484F-483A-85AB-A1760D5409A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+  <si>
+    <t>Farmer Table</t>
+  </si>
+  <si>
+    <t>Property Name</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Farmer Id</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Primary Key</t>
+  </si>
+  <si>
+    <t>Not Null</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Big Int</t>
+  </si>
+  <si>
+    <t>Mail Id</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -37,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +112,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +417,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Database schema updated by Pratik
</commit_message>
<xml_diff>
--- a/doc/Database schema.xlsx
+++ b/doc/Database schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pratik CDAC\Project\Online-Bidding-system-Group-19-Project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDD9BD-484F-483A-85AB-A1760D5409A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D83CFBA-54AC-4F7F-87E4-B070BD17CA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>Farmer Table</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Buyer Table</t>
+  </si>
+  <si>
+    <t>Buyer Id</t>
+  </si>
+  <si>
+    <t>Admin Table</t>
+  </si>
+  <si>
+    <t>Admin Id</t>
   </si>
 </sst>
 </file>
@@ -418,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,9 +530,183 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
database schema updayed by Pratik
</commit_message>
<xml_diff>
--- a/doc/Database schema.xlsx
+++ b/doc/Database schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pratik CDAC\Project\Online-Bidding-system-Group-19-Project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D83CFBA-54AC-4F7F-87E4-B070BD17CA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA990779-E8F9-4FC1-867D-9F6060B6E5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
   <si>
     <t>Farmer Table</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Admin Id</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Unique Key</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -143,13 +152,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,75 +540,81 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -608,83 +624,83 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>10</v>
@@ -694,19 +710,39 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>